<commit_message>
v2.0.0 RC1 - added excel log; added case list viewer and search based on excel logged cases. added search logic to find local powerpoint to open file via cmd;
</commit_message>
<xml_diff>
--- a/Resources/MyCaseLogTemplate.xlsx
+++ b/Resources/MyCaseLogTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kartuzv\source\repos\MyCaseLog\LogArchive\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kartuzv\source\repos\MyCaseLog\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,27 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>LogID</t>
   </si>
   <si>
-    <t>Hospital</t>
-  </si>
-  <si>
-    <t>Modality</t>
-  </si>
-  <si>
     <t>BodyPart</t>
-  </si>
-  <si>
-    <t>Protocol</t>
-  </si>
-  <si>
-    <t>Sex</t>
-  </si>
-  <si>
-    <t>Age</t>
   </si>
   <si>
     <t>Accession</t>
@@ -56,22 +41,16 @@
     <t>MRN</t>
   </si>
   <si>
-    <t>POI</t>
+    <t>Notes</t>
   </si>
   <si>
-    <t>LocalConf</t>
+    <t>Speciality</t>
   </si>
   <si>
-    <t>SocietyConf</t>
+    <t>Tags</t>
   </si>
   <si>
-    <t>ManuscriptPublished</t>
-  </si>
-  <si>
-    <t>DollarAmount</t>
-  </si>
-  <si>
-    <t>CaseFolder</t>
+    <t>PowerPointFile</t>
   </si>
 </sst>
 </file>
@@ -89,7 +68,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -109,7 +88,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -132,38 +111,552 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -174,6 +667,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H1048576" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9" totalsRowBorderDxfId="8">
+  <autoFilter ref="A1:H1048576"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="LogID" dataDxfId="7"/>
+    <tableColumn id="2" name="Speciality" dataDxfId="6"/>
+    <tableColumn id="3" name="BodyPart" dataDxfId="5"/>
+    <tableColumn id="4" name="Accession" dataDxfId="4"/>
+    <tableColumn id="5" name="MRN" dataDxfId="3"/>
+    <tableColumn id="6" name="Notes" dataDxfId="2"/>
+    <tableColumn id="7" name="Tags" dataDxfId="1"/>
+    <tableColumn id="8" name="PowerPointFile" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -439,77 +949,57 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.5703125" style="1" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6" style="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="34.42578125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="8.140625" style="4" customWidth="1"/>
-    <col min="12" max="13" width="9.140625" style="4" customWidth="1"/>
-    <col min="14" max="14" width="11" style="3" customWidth="1"/>
-    <col min="15" max="15" width="23.5703125" style="1" customWidth="1"/>
-    <col min="16" max="20" width="9.140625" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="17.5703125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="37" style="9" customWidth="1"/>
+    <col min="7" max="7" width="50.140625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="24.140625" style="10" customWidth="1"/>
+    <col min="9" max="13" width="9.140625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>